<commit_message>
adding CVRMSE and NMBE as reporting variables
</commit_message>
<xml_diff>
--- a/projects/office_calibration_nsga2.xlsx
+++ b/projects/office_calibration_nsga2.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2618" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2634" uniqueCount="845">
   <si>
     <t>type</t>
   </si>
@@ -2552,6 +2552,30 @@
   </si>
   <si>
     <t>O &amp; M Frequency</t>
+  </si>
+  <si>
+    <t>calibration_reports.electric_bill_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports.electric_bill_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports.gas_bill_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports.gas_bill_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>Electric CVRMSE</t>
+  </si>
+  <si>
+    <t>Electric NMBE</t>
+  </si>
+  <si>
+    <t>Gas CVRMSE</t>
+  </si>
+  <si>
+    <t>Gas NMBE</t>
   </si>
 </sst>
 </file>
@@ -10279,9 +10303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11171,28 +11195,100 @@
       <c r="L28" s="30"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="30"/>
+      <c r="A29" s="30" t="s">
+        <v>841</v>
+      </c>
       <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="30" t="s">
+        <v>837</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
+      <c r="A30" s="30" t="s">
+        <v>842</v>
+      </c>
       <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="30" t="s">
+        <v>838</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
+      <c r="A31" s="30" t="s">
+        <v>843</v>
+      </c>
       <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="30" t="s">
+        <v>839</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
+      <c r="A32" s="30" t="s">
+        <v>844</v>
+      </c>
       <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
+      <c r="C32" s="30" t="s">
+        <v>840</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="30"/>
@@ -11220,7 +11316,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>